<commit_message>
feat: write test.py to paste template
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="32">
   <si>
     <r>
       <rPr>
@@ -266,6 +266,18 @@
       </rPr>
       <t>9A</t>
     </r>
+  </si>
+  <si>
+    <t>2310-P-02161-B62SA0</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>4270</t>
+  </si>
+  <si>
+    <t>16</t>
   </si>
 </sst>
 </file>
@@ -278,7 +290,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,13 +310,6 @@
       <color rgb="FF000000"/>
       <name val="楷体"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -987,48 +992,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1038,97 +1046,94 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1503,10 +1508,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1965,7 +1970,39 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" ht="15"/>
+    <row r="15" ht="27" spans="1:10">
+      <c r="A15" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" ht="15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>